<commit_message>
Added solution (checklists) for task 1.
</commit_message>
<xml_diff>
--- a/Check lists/Check List_1.xlsx
+++ b/Check lists/Check List_1.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Search Field" sheetId="2" r:id="rId2"/>
+    <sheet name="Search Results" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Search field:</t>
   </si>
@@ -48,13 +48,275 @@
   </si>
   <si>
     <t>Task:</t>
+  </si>
+  <si>
+    <t>Checklist for the Search Field:</t>
+  </si>
+  <si>
+    <t>Status:</t>
+  </si>
+  <si>
+    <t>Bug link:</t>
+  </si>
+  <si>
+    <t>Verify that you can go to www.search.com/</t>
+  </si>
+  <si>
+    <t>Pre-conditions:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You are went to https://www.search.com/ </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that  the search page contains correct elements after loading </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(title "Search",  magnifying glass image, button "SEARCH", search field)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Verify that there is a title "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>" above the search field</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that there is a magnifying glass image under the title "Search" and above the search field</t>
+  </si>
+  <si>
+    <r>
+      <t>Verify that  the search button on the right of the search field with the text "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>SEARCH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>"</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that the title "Search" has a correct style</t>
+  </si>
+  <si>
+    <r>
+      <t>Verify that the button "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>SEARCH</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>" has a correct style</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that the search field is active when you click on it</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that you can enter letters in the search field </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(e.g. Star Trek)</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that user can search with letters</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that you can enter numbers in the search field </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>(e.g. 1234567890)</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that user can search with numbers</t>
+  </si>
+  <si>
+    <t>Verify that  you can't enter characters as !, @, #, $, %, ^, &amp;, *, (, ?</t>
+  </si>
+  <si>
+    <r>
+      <t>Verify that user can search with a combination of characters in the search field</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (e.g. Oscar 2016)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that you can enter a valid phrase with a &lt;40 characters in the search field </t>
+  </si>
+  <si>
+    <t>Verify that you can enter a valid phrase with a &lt;40 characters in the search field using CTRL+V in the search field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user can search with a valid phrase with a &lt;40 characters in the search field </t>
+  </si>
+  <si>
+    <t>Verify that you can't enter a valid phrase with a &gt;40 characters in the search field</t>
+  </si>
+  <si>
+    <t>Verify that only the first 40 characters are displayed in the search field, when you try to enter a valid phrase with a &gt;40 characters</t>
+  </si>
+  <si>
+    <t>Verify that only the first 40 characters are displayed in the search field, when you try to enter a valid phrase with a &gt;40 characters using CTRL+V</t>
+  </si>
+  <si>
+    <t>Verify that you can click on the button "search"</t>
+  </si>
+  <si>
+    <t>Verify that the search results page is loading</t>
+  </si>
+  <si>
+    <t>Verify that if user clicks on the button "search" without search term in the search field, then the user does not go to the search results page and nothing happens</t>
+  </si>
+  <si>
+    <t>Checklist for the Search Results page:</t>
+  </si>
+  <si>
+    <t>You are went to https://www.search.com/, clicked on the search field, enter a search term in the search field and clicked on the button "search"</t>
+  </si>
+  <si>
+    <r>
+      <t>Verify that user can see a message "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>No results found for this term</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>" when performing a search if there aren't  results for this query</t>
+    </r>
+  </si>
+  <si>
+    <t>Verify that  the search results are relevant</t>
+  </si>
+  <si>
+    <t>Verify that the search results are displayed in the list format</t>
+  </si>
+  <si>
+    <t>Verify that the user can use the page scroll bar</t>
+  </si>
+  <si>
+    <t>Verify that the user can go to the next page of search results</t>
+  </si>
+  <si>
+    <t>Verify that the user can return to the search page after  searching and  search for something else by using the back button of the browser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,8 +339,37 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,8 +388,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -121,11 +418,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -140,6 +509,68 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -473,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -541,24 +972,396 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <v>3</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <v>5</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="27">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <v>8</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <v>9</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
+        <v>10</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="27">
+        <v>11</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <v>12</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <v>13</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="27">
+        <v>14</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <v>15</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="27">
+        <v>16</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="27">
+        <v>17</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="27">
+        <v>18</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="27">
+        <v>19</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="27">
+        <v>20</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="27">
+        <v>21</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="27">
+        <v>22</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="15"/>
+    </row>
+    <row r="3" spans="1:4" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
+        <v>5</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>